<commit_message>
created new location Qr report and multiselect fields for people,asset and checjpoint Qr reports.
</commit_message>
<xml_diff>
--- a/docs/caps.xlsx
+++ b/docs/caps.xlsx
@@ -749,11 +749,11 @@
   </sheetPr>
   <dimension ref="A1:E103"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E86" activeCellId="0" sqref="E86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="31.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="32.44"/>

</xml_diff>

<commit_message>
changes in shift | Dashboard | sidebar | Contract Form and List | Manohar
</commit_message>
<xml_diff>
--- a/docs/caps.xlsx
+++ b/docs/caps.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="204">
   <si>
     <t>ID</t>
   </si>
@@ -614,6 +614,12 @@
   </si>
   <si>
     <t>Static Tour Details</t>
+  </si>
+  <si>
+    <t>OB_CS_CONTRACTDETAILS</t>
+  </si>
+  <si>
+    <t>Contract Details</t>
   </si>
   <si>
     <t>RP_SITEVISITREPORT</t>
@@ -637,7 +643,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -676,7 +682,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -688,7 +694,13 @@
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -992,20 +1004,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E103"/>
+  <dimension ref="A1:E104"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="31.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="31.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="32.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="18.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="31.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="31.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="32.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="18.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1022,7 +1034,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="3"/>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -1037,7 +1049,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="3"/>
       <c r="B3" s="1" t="s">
         <v>9</v>
@@ -1052,7 +1064,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="3"/>
       <c r="B4" s="1" t="s">
         <v>12</v>
@@ -1067,7 +1079,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="3"/>
       <c r="B5" s="1" t="s">
         <v>14</v>
@@ -1082,7 +1094,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="3"/>
       <c r="B6" s="1" t="s">
         <v>16</v>
@@ -1097,7 +1109,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="3"/>
       <c r="B7" s="1" t="s">
         <v>18</v>
@@ -1112,7 +1124,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="3"/>
       <c r="B8" s="1" t="s">
         <v>20</v>
@@ -1127,7 +1139,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="3"/>
       <c r="B9" s="1" t="s">
         <v>22</v>
@@ -1142,7 +1154,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="3"/>
       <c r="B10" s="1" t="s">
         <v>24</v>
@@ -1157,7 +1169,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="3"/>
       <c r="B11" s="1" t="s">
         <v>26</v>
@@ -1172,7 +1184,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="3"/>
       <c r="B12" s="1" t="s">
         <v>28</v>
@@ -1187,7 +1199,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="3"/>
       <c r="B13" s="1" t="s">
         <v>30</v>
@@ -1202,7 +1214,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="3"/>
       <c r="B14" s="1" t="s">
         <v>32</v>
@@ -1217,7 +1229,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="3"/>
       <c r="B15" s="1" t="s">
         <v>34</v>
@@ -1232,7 +1244,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="3"/>
       <c r="B16" s="1" t="s">
         <v>36</v>
@@ -1247,7 +1259,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="3"/>
       <c r="B17" s="1" t="s">
         <v>38</v>
@@ -1262,7 +1274,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="3"/>
       <c r="B18" s="1" t="s">
         <v>40</v>
@@ -1277,7 +1289,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="3"/>
       <c r="B19" s="1" t="s">
         <v>42</v>
@@ -1292,7 +1304,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="3"/>
       <c r="B20" s="1" t="s">
         <v>44</v>
@@ -1307,7 +1319,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="3"/>
       <c r="B21" s="1" t="s">
         <v>46</v>
@@ -1322,7 +1334,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="3"/>
       <c r="B22" s="1" t="s">
         <v>48</v>
@@ -1337,7 +1349,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="3"/>
       <c r="B23" s="1" t="s">
         <v>50</v>
@@ -1352,7 +1364,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="3"/>
       <c r="B24" s="1" t="s">
         <v>52</v>
@@ -2539,16 +2551,31 @@
     </row>
     <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="17.25">
       <c r="A103" s="3"/>
-      <c r="B103" s="1" t="s">
+      <c r="B103" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="C103" s="1" t="s">
+      <c r="C103" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="D103" s="1" t="s">
+      <c r="D103" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E103" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="17.25">
+      <c r="A104" s="3"/>
+      <c r="B104" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D104" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="E103" s="1" t="s">
+      <c r="E104" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>